<commit_message>
Committing changes in excel
</commit_message>
<xml_diff>
--- a/Mendix/input/data/Local_Material_Data.xlsx
+++ b/Mendix/input/data/Local_Material_Data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="82">
   <si>
     <t>S.NO</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>2, Transfer</t>
+  </si>
+  <si>
+    <t>0.001</t>
   </si>
 </sst>
 </file>
@@ -715,7 +718,7 @@
   <dimension ref="A1:IX3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -803,7 +806,7 @@
         <v>57</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>71</v>
@@ -856,7 +859,7 @@
         <v>57</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>71</v>
@@ -871,7 +874,7 @@
         <v>72</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>72</v>

</xml_diff>